<commit_message>
Updated PCB and added 3D view
</commit_message>
<xml_diff>
--- a/BOM/BOM_weather_station.xlsx
+++ b/BOM/BOM_weather_station.xlsx
@@ -1171,7 +1171,7 @@
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1203,12 +1203,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
@@ -1230,6 +1224,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1492,11 +1487,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1553,47 +1548,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1613,7 +1604,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1633,7 +1624,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1780,11 +1771,11 @@
   </sheetPr>
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="41.57"/>
@@ -1792,7 +1783,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="70.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="93.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="26.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.52"/>
@@ -1912,16 +1903,16 @@
       <c r="J11" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="K11" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="14" t="s">
+      <c r="L11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="14" t="s">
+      <c r="M11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="N11" s="14" t="s">
+      <c r="N11" s="13" t="s">
         <v>25</v>
       </c>
       <c r="O11" s="13" t="s">
@@ -1971,7 +1962,7 @@
       <c r="N12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="O12" s="15" t="s">
+      <c r="O12" s="14" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2018,7 +2009,7 @@
       <c r="N13" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="14" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2065,7 +2056,7 @@
       <c r="N14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="O14" s="15" t="s">
+      <c r="O14" s="14" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2112,7 +2103,7 @@
       <c r="N15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="O15" s="15" t="s">
+      <c r="O15" s="14" t="s">
         <v>56</v>
       </c>
     </row>
@@ -2159,7 +2150,7 @@
       <c r="N16" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="O16" s="15" t="s">
+      <c r="O16" s="14" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2206,7 +2197,7 @@
       <c r="N17" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="O17" s="15" t="s">
+      <c r="O17" s="14" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2253,7 +2244,7 @@
       <c r="N18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="O18" s="15" t="s">
+      <c r="O18" s="14" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2300,7 +2291,7 @@
       <c r="N19" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="O19" s="15" t="s">
+      <c r="O19" s="14" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2347,7 +2338,7 @@
       <c r="N20" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="O20" s="15" t="s">
+      <c r="O20" s="14" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2394,7 +2385,7 @@
       <c r="N21" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="O21" s="15" t="s">
+      <c r="O21" s="14" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2441,7 +2432,7 @@
       <c r="N22" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="O22" s="15" t="s">
+      <c r="O22" s="14" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2488,7 +2479,7 @@
       <c r="N23" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="O23" s="15" t="s">
+      <c r="O23" s="14" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2535,7 +2526,7 @@
       <c r="N24" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="O24" s="15" t="s">
+      <c r="O24" s="14" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2582,7 +2573,7 @@
       <c r="N25" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="O25" s="15" t="s">
+      <c r="O25" s="14" t="s">
         <v>145</v>
       </c>
     </row>
@@ -2629,7 +2620,7 @@
       <c r="N26" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="O26" s="15" t="s">
+      <c r="O26" s="14" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2676,7 +2667,7 @@
       <c r="N27" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="O27" s="15" t="s">
+      <c r="O27" s="14" t="s">
         <v>166</v>
       </c>
     </row>
@@ -2723,7 +2714,7 @@
       <c r="N28" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="O28" s="15" t="s">
+      <c r="O28" s="14" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2770,7 +2761,7 @@
       <c r="N29" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="O29" s="15" t="s">
+      <c r="O29" s="14" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2817,7 +2808,7 @@
       <c r="N30" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="O30" s="15" t="s">
+      <c r="O30" s="14" t="s">
         <v>187</v>
       </c>
     </row>
@@ -2864,7 +2855,7 @@
       <c r="N31" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="O31" s="15" t="s">
+      <c r="O31" s="14" t="s">
         <v>193</v>
       </c>
     </row>
@@ -2911,7 +2902,7 @@
       <c r="N32" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="O32" s="15" t="s">
+      <c r="O32" s="14" t="s">
         <v>199</v>
       </c>
     </row>
@@ -2958,7 +2949,7 @@
       <c r="N33" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="O33" s="15" t="s">
+      <c r="O33" s="14" t="s">
         <v>205</v>
       </c>
     </row>
@@ -3005,7 +2996,7 @@
       <c r="N34" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="O34" s="15" t="s">
+      <c r="O34" s="14" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3052,7 +3043,7 @@
       <c r="N35" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="O35" s="15" t="s">
+      <c r="O35" s="14" t="s">
         <v>217</v>
       </c>
     </row>
@@ -3099,7 +3090,7 @@
       <c r="N36" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="O36" s="15" t="s">
+      <c r="O36" s="14" t="s">
         <v>223</v>
       </c>
     </row>
@@ -3146,7 +3137,7 @@
       <c r="N37" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="O37" s="15" t="s">
+      <c r="O37" s="14" t="s">
         <v>229</v>
       </c>
     </row>
@@ -3193,7 +3184,7 @@
       <c r="N38" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="O38" s="15" t="s">
+      <c r="O38" s="14" t="s">
         <v>234</v>
       </c>
     </row>
@@ -3240,7 +3231,7 @@
       <c r="N39" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="O39" s="15" t="s">
+      <c r="O39" s="14" t="s">
         <v>239</v>
       </c>
     </row>
@@ -3287,7 +3278,7 @@
       <c r="N40" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="O40" s="15" t="s">
+      <c r="O40" s="14" t="s">
         <v>242</v>
       </c>
     </row>
@@ -3334,7 +3325,7 @@
       <c r="N41" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="O41" s="15" t="s">
+      <c r="O41" s="14" t="s">
         <v>253</v>
       </c>
     </row>
@@ -3381,7 +3372,7 @@
       <c r="N42" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="O42" s="15" t="s">
+      <c r="O42" s="14" t="s">
         <v>263</v>
       </c>
     </row>
@@ -3428,7 +3419,7 @@
       <c r="N43" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="O43" s="15" t="s">
+      <c r="O43" s="14" t="s">
         <v>273</v>
       </c>
     </row>
@@ -3475,7 +3466,7 @@
       <c r="N44" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="O44" s="15" t="s">
+      <c r="O44" s="14" t="s">
         <v>284</v>
       </c>
     </row>
@@ -3522,7 +3513,7 @@
       <c r="N45" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="O45" s="15" t="s">
+      <c r="O45" s="14" t="s">
         <v>293</v>
       </c>
     </row>
@@ -3569,7 +3560,7 @@
       <c r="N46" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="O46" s="15" t="s">
+      <c r="O46" s="14" t="s">
         <v>303</v>
       </c>
     </row>
@@ -3616,7 +3607,7 @@
       <c r="N47" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="O47" s="15" t="s">
+      <c r="O47" s="14" t="s">
         <v>313</v>
       </c>
     </row>
@@ -3663,7 +3654,7 @@
       <c r="N48" s="10" t="s">
         <v>323</v>
       </c>
-      <c r="O48" s="15" t="s">
+      <c r="O48" s="14" t="s">
         <v>324</v>
       </c>
     </row>
@@ -3710,7 +3701,7 @@
       <c r="N49" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="O49" s="15" t="s">
+      <c r="O49" s="14" t="s">
         <v>334</v>
       </c>
     </row>
@@ -3757,7 +3748,7 @@
       <c r="N50" s="10" t="s">
         <v>343</v>
       </c>
-      <c r="O50" s="15" t="s">
+      <c r="O50" s="14" t="s">
         <v>344</v>
       </c>
     </row>
@@ -3804,7 +3795,7 @@
       <c r="N51" s="10" t="s">
         <v>352</v>
       </c>
-      <c r="O51" s="15" t="s">
+      <c r="O51" s="14" t="s">
         <v>353</v>
       </c>
     </row>
@@ -3847,119 +3838,119 @@
       <c r="N52" s="10" t="s">
         <v>359</v>
       </c>
-      <c r="O52" s="15" t="s">
+      <c r="O52" s="14" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H55" s="16" t="s">
+      <c r="H55" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="I55" s="17" t="s">
+      <c r="I55" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="J55" s="17"/>
-      <c r="K55" s="18" t="s">
+      <c r="J55" s="16"/>
+      <c r="K55" s="17" t="s">
         <v>363</v>
       </c>
-      <c r="L55" s="18"/>
-      <c r="M55" s="17" t="s">
+      <c r="L55" s="17"/>
+      <c r="M55" s="16" t="s">
         <v>364</v>
       </c>
-      <c r="N55" s="17"/>
+      <c r="N55" s="16"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H56" s="16"/>
-      <c r="I56" s="19" t="s">
+      <c r="H56" s="15"/>
+      <c r="I56" s="18" t="s">
         <v>365</v>
       </c>
-      <c r="J56" s="20" t="s">
+      <c r="J56" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="K56" s="21" t="s">
+      <c r="K56" s="20" t="s">
         <v>365</v>
       </c>
-      <c r="L56" s="22" t="s">
+      <c r="L56" s="21" t="s">
         <v>366</v>
       </c>
-      <c r="M56" s="23" t="s">
+      <c r="M56" s="22" t="s">
         <v>365</v>
       </c>
-      <c r="N56" s="20" t="s">
+      <c r="N56" s="19" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H57" s="24" t="s">
+      <c r="H57" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="I57" s="25" t="s">
+      <c r="I57" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="J57" s="25" t="s">
+      <c r="J57" s="24" t="s">
         <v>368</v>
       </c>
-      <c r="K57" s="26" t="s">
+      <c r="K57" s="25" t="s">
         <v>369</v>
       </c>
-      <c r="L57" s="27" t="s">
+      <c r="L57" s="26" t="s">
         <v>370</v>
       </c>
-      <c r="M57" s="25" t="s">
+      <c r="M57" s="24" t="s">
         <v>371</v>
       </c>
-      <c r="N57" s="28" t="s">
+      <c r="N57" s="27" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H58" s="29" t="s">
+      <c r="H58" s="28" t="s">
         <v>373</v>
       </c>
-      <c r="I58" s="30" t="s">
+      <c r="I58" s="29" t="s">
         <v>374</v>
       </c>
-      <c r="J58" s="30" t="s">
+      <c r="J58" s="29" t="s">
         <v>374</v>
       </c>
-      <c r="K58" s="31" t="s">
+      <c r="K58" s="30" t="s">
         <v>375</v>
       </c>
-      <c r="L58" s="32" t="s">
+      <c r="L58" s="31" t="s">
         <v>376</v>
       </c>
-      <c r="M58" s="30" t="s">
+      <c r="M58" s="29" t="s">
         <v>377</v>
       </c>
-      <c r="N58" s="33" t="s">
+      <c r="N58" s="32" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H59" s="34" t="s">
+      <c r="H59" s="33" t="s">
         <v>379</v>
       </c>
-      <c r="I59" s="35" t="str">
+      <c r="I59" s="34" t="str">
         <f aca="false">_xlfn.CONCAT(SUM(SUBSTITUTE(I57, " zł", ""), SUBSTITUTE(I58, " zł", "")), " zł")</f>
         <v>366.59 zł</v>
       </c>
-      <c r="J59" s="35" t="str">
+      <c r="J59" s="34" t="str">
         <f aca="false">_xlfn.CONCAT(SUM(SUBSTITUTE(J57, " zł", ""), SUBSTITUTE(J58, " zł", "")), " zł")</f>
         <v>366.59 zł</v>
       </c>
-      <c r="K59" s="36" t="str">
+      <c r="K59" s="35" t="str">
         <f aca="false">_xlfn.CONCAT(SUM(SUBSTITUTE(K57, " zł", ""), SUBSTITUTE(K58, " zł", "")), " zł")</f>
         <v>3251.77 zł</v>
       </c>
-      <c r="L59" s="37" t="str">
+      <c r="L59" s="36" t="str">
         <f aca="false">_xlfn.CONCAT(SUM(SUBSTITUTE(L57, " zł", ""), SUBSTITUTE(L58, " zł", "")), " zł")</f>
         <v>298.57 zł</v>
       </c>
-      <c r="M59" s="35" t="str">
+      <c r="M59" s="34" t="str">
         <f aca="false">_xlfn.CONCAT(SUM(SUBSTITUTE(M57, " zł", ""), SUBSTITUTE(M58, " zł", "")), " zł")</f>
         <v>26145.02 zł</v>
       </c>
-      <c r="N59" s="38" t="str">
+      <c r="N59" s="37" t="str">
         <f aca="false">_xlfn.CONCAT(SUM(SUBSTITUTE(N57, " zł", ""), SUBSTITUTE(N58, " zł", "")), " zł")</f>
         <v>252.06 zł</v>
       </c>

</xml_diff>